<commit_message>
change column names SAMPLESHEET_TO_BARCODE
</commit_message>
<xml_diff>
--- a/tests/data/samplesheets/clip-samplesheet.xlsx
+++ b/tests/data/samplesheets/clip-samplesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cheshic/dev/repos/goodwright/flow-nf/tests/data/samplesheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/capitac/repos/flow-nf/tests/data/samplesheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F890BBF-FEB7-5C4B-BA22-87239AC70AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3C4EE3-F109-8446-9305-6B742AE47ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="500" windowWidth="28040" windowHeight="16400"/>
+    <workbookView xWindow="160" yWindow="760" windowWidth="28040" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clip-samplesheet" sheetId="1" r:id="rId1"/>
@@ -21,15 +21,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>5prime_barcode</t>
-  </si>
-  <si>
-    <t>3prime_barcode</t>
-  </si>
   <si>
     <t>adapter_sequence</t>
   </si>
@@ -51,11 +42,20 @@
   <si>
     <t>NNNTTGTNN</t>
   </si>
+  <si>
+    <t>Sample Name</t>
+  </si>
+  <si>
+    <t>5' Barcode Sequence</t>
+  </si>
+  <si>
+    <t>3' Barcode Sequence</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -889,50 +889,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="A1:G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Demultiplex now supports multiple samplesheets
</commit_message>
<xml_diff>
--- a/tests/data/samplesheets/clip-samplesheet.xlsx
+++ b/tests/data/samplesheets/clip-samplesheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cheshic/dev/repos/goodwright/flow-nf/tests/data/samplesheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6D19BE-F1E7-6C4A-9BB4-434BED514170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31D61BB-5D78-934A-A30A-C214ACAD6F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Sample1</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>3' Adapter Sequence</t>
+  </si>
+  <si>
+    <t>NNGACNN</t>
   </si>
 </sst>
 </file>
@@ -916,7 +919,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,6 +951,9 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>

</xml_diff>